<commit_message>
updated charts in kruskal
</commit_message>
<xml_diff>
--- a/charakterystyka.xlsx
+++ b/charakterystyka.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="CHOR1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="CHOR2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="KONTROLA" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">group_name</t>
   </si>
@@ -61,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">CHOR2 med</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KONTROLA sr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KONTROLA os</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KONTROLA med</t>
   </si>
 </sst>
 </file>
@@ -435,7 +445,7 @@
         <v>6.1</v>
       </c>
       <c r="D2" t="n">
-        <v>4.17</v>
+        <v>5.36</v>
       </c>
       <c r="E2" t="n">
         <v>225.28</v>
@@ -450,7 +460,7 @@
         <v>35.13</v>
       </c>
       <c r="I2" t="n">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
       <c r="J2" t="n">
         <v>12.02</v>
@@ -467,7 +477,7 @@
         <v>8.82</v>
       </c>
       <c r="D3" t="n">
-        <v>0.38</v>
+        <v>5.77</v>
       </c>
       <c r="E3" t="n">
         <v>54.22</v>
@@ -482,7 +492,7 @@
         <v>0.88</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="J3" t="n">
         <v>2.58</v>
@@ -499,7 +509,7 @@
         <v>3.97</v>
       </c>
       <c r="D4" t="n">
-        <v>4.19</v>
+        <v>4.2</v>
       </c>
       <c r="E4" t="n">
         <v>217</v>
@@ -577,7 +587,7 @@
         <v>6.1</v>
       </c>
       <c r="D2" t="n">
-        <v>4.17</v>
+        <v>5.36</v>
       </c>
       <c r="E2" t="n">
         <v>225.28</v>
@@ -592,7 +602,7 @@
         <v>35.13</v>
       </c>
       <c r="I2" t="n">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
       <c r="J2" t="n">
         <v>12.02</v>
@@ -609,7 +619,7 @@
         <v>8.82</v>
       </c>
       <c r="D3" t="n">
-        <v>0.38</v>
+        <v>5.77</v>
       </c>
       <c r="E3" t="n">
         <v>54.22</v>
@@ -624,7 +634,7 @@
         <v>0.88</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="J3" t="n">
         <v>2.58</v>
@@ -641,7 +651,149 @@
         <v>3.97</v>
       </c>
       <c r="D4" t="n">
-        <v>4.19</v>
+        <v>4.2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>217</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="H4" t="n">
+        <v>35.05</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="J4" t="n">
+        <v>11.66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="n">
+        <v>29.56</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.36</v>
+      </c>
+      <c r="E2" t="n">
+        <v>225.28</v>
+      </c>
+      <c r="F2" t="n">
+        <v>12.41</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="H2" t="n">
+        <v>35.13</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="J2" t="n">
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8.82</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5.77</v>
+      </c>
+      <c r="E3" t="n">
+        <v>54.22</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="n">
+        <v>29</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4.2</v>
       </c>
       <c r="E4" t="n">
         <v>217</v>

</xml_diff>